<commit_message>
remove autmomated code generation
</commit_message>
<xml_diff>
--- a/server/resource/excel/ExcelExport.xlsx
+++ b/server/resource/excel/ExcelExport.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89B7DE-2C93-48FD-8CEC-AB113C1A539A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -44,69 +45,24 @@
   </si>
   <si>
     <t>/</t>
-  </si>
-  <si>
-    <t>dashboard</t>
-  </si>
-  <si>
-    <t>view/dashboard/index.vue</t>
-  </si>
-  <si>
-    <t>superAdmin</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>view/superAdmin/index.vue</t>
-  </si>
-  <si>
-    <t>person</t>
-  </si>
-  <si>
-    <t>view/person/person.vue</t>
-  </si>
-  <si>
-    <t>systemTools</t>
-  </si>
-  <si>
-    <t>view/systemTools/index.vue</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>view/system/state.vue</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>view/example/index.vue</t>
-  </si>
-  <si>
-    <t>about</t>
-  </si>
-  <si>
-    <t>view/about/index.vue</t>
-  </si>
-  <si>
-    <t>Wakty</t>
-  </si>
-  <si>
-    <t>view/routerHolder.vue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,10 +89,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,14 +361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="A3:I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,9 +393,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -450,190 +416,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>900</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>